<commit_message>
Rename 7_or_more_percent to fail_percent
</commit_message>
<xml_diff>
--- a/global-player-stats.xlsx
+++ b/global-player-stats.xlsx
@@ -49,7 +49,7 @@
     <t>6_try_percent</t>
   </si>
   <si>
-    <t>7_or_more_percent</t>
+    <t>fail_percent</t>
   </si>
   <si>
     <t>manly</t>
@@ -1134,13 +1134,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1190,8 +1196,8 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -8141,7 +8147,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="18.75">
       <c r="A175" s="1">
         <v>44753</v>
       </c>
@@ -8179,7 +8185,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="18.75">
       <c r="A176" s="1">
         <v>44752</v>
       </c>
@@ -8217,7 +8223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="18.75">
       <c r="A177" s="1">
         <v>44751</v>
       </c>
@@ -8255,7 +8261,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="18.75">
       <c r="A178" s="1">
         <v>44750</v>
       </c>
@@ -8293,7 +8299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="18.75">
       <c r="A179" s="1">
         <v>44749</v>
       </c>
@@ -8331,7 +8337,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="18.75">
       <c r="A180" s="1">
         <v>44748</v>
       </c>
@@ -8369,7 +8375,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="18.75">
       <c r="A181" s="1">
         <v>44747</v>
       </c>
@@ -8407,7 +8413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="182" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="182" customHeight="1" ht="18.75">
       <c r="A182" s="1">
         <v>44746</v>
       </c>
@@ -8445,7 +8451,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="183" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="183" customHeight="1" ht="18.75">
       <c r="A183" s="1">
         <v>44745</v>
       </c>
@@ -8483,7 +8489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="18.75">
       <c r="A184" s="1">
         <v>44744</v>
       </c>
@@ -8521,7 +8527,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="18.75">
       <c r="A185" s="1">
         <v>44743</v>
       </c>
@@ -8559,7 +8565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="186" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="186" customHeight="1" ht="18.75">
       <c r="A186" s="1">
         <v>44742</v>
       </c>
@@ -8597,7 +8603,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="187" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="187" customHeight="1" ht="18.75">
       <c r="A187" s="1">
         <v>44741</v>
       </c>
@@ -8635,7 +8641,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="188" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="188" customHeight="1" ht="18.75">
       <c r="A188" s="1">
         <v>44740</v>
       </c>
@@ -8673,7 +8679,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="189" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="189" customHeight="1" ht="18.75">
       <c r="A189" s="1">
         <v>44739</v>
       </c>
@@ -8711,7 +8717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="190" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="190" customHeight="1" ht="18.75">
       <c r="A190" s="1">
         <v>44738</v>
       </c>
@@ -8749,7 +8755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="191" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="191" customHeight="1" ht="18.75">
       <c r="A191" s="1">
         <v>44737</v>
       </c>
@@ -8787,7 +8793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="18.75">
       <c r="A192" s="1">
         <v>44736</v>
       </c>
@@ -8825,7 +8831,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="18.75">
       <c r="A193" s="1">
         <v>44735</v>
       </c>
@@ -8863,7 +8869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="194" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="194" customHeight="1" ht="18.75">
       <c r="A194" s="1">
         <v>44734</v>
       </c>
@@ -8901,7 +8907,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="195" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="195" customHeight="1" ht="18.75">
       <c r="A195" s="1">
         <v>44733</v>
       </c>
@@ -8939,7 +8945,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="196" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="196" customHeight="1" ht="18.75">
       <c r="A196" s="1">
         <v>44732</v>
       </c>
@@ -8977,7 +8983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="197" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="197" customHeight="1" ht="18.75">
       <c r="A197" s="1">
         <v>44731</v>
       </c>
@@ -9015,7 +9021,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="198" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="198" customHeight="1" ht="18.75">
       <c r="A198" s="1">
         <v>44730</v>
       </c>
@@ -9053,7 +9059,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="199" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="199" customHeight="1" ht="18.75">
       <c r="A199" s="1">
         <v>44729</v>
       </c>
@@ -9091,7 +9097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="200" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="200" customHeight="1" ht="18.75">
       <c r="A200" s="1">
         <v>44728</v>
       </c>
@@ -9129,7 +9135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="201" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="201" customHeight="1" ht="18.75">
       <c r="A201" s="1">
         <v>44727</v>
       </c>

</xml_diff>